<commit_message>
Add a new analyte class: Lipid + metabolite + protein
Closes #143
</commit_message>
<xml_diff>
--- a/mplex/latest/mplex.xlsx
+++ b/mplex/latest/mplex.xlsx
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="526">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -460,6 +460,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
+    <t>iCLAP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000479</t>
+  </si>
+  <si>
     <t>seqFISH</t>
   </si>
   <si>
@@ -709,6 +715,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C13201</t>
   </si>
   <si>
+    <t>Lipid + metabolite + protein</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000478</t>
+  </si>
+  <si>
     <t>RNA + protein</t>
   </si>
   <si>
@@ -895,6 +907,12 @@
     <t>https://identifiers.org/RRID:SCR_023605</t>
   </si>
   <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024589</t>
+  </si>
+  <si>
     <t>In-House</t>
   </si>
   <si>
@@ -1090,6 +1108,12 @@
     <t>https://identifiers.org/RRID:SCR_026452</t>
   </si>
   <si>
+    <t>DMi8</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026672</t>
+  </si>
+  <si>
     <t>Opera Phenix Plus HCS</t>
   </si>
   <si>
@@ -1270,6 +1294,12 @@
     <t>https://identifiers.org/RRID:SCR_027072</t>
   </si>
   <si>
+    <t>Opera Phenix HCS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027817</t>
+  </si>
+  <si>
     <t>Zeiss LightSheet Z.1</t>
   </si>
   <si>
@@ -1726,12 +1756,6 @@
     <t>https://identifiers.org/RRID:SCR_013575</t>
   </si>
   <si>
-    <t>Waters</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024589</t>
-  </si>
-  <si>
     <t>lc_instrument_model</t>
   </si>
   <si>
@@ -1903,7 +1927,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-12-15T11:36:24-08:00</t>
+    <t>2026-02-05T10:17:35-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2091,156 +2115,156 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AT2" t="s" s="47">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="32">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$53</formula1>
+      <formula1>'dataset_type'!$A$1:$A$54</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$17</formula1>
+      <formula1>'analyte_class'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$31</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$32</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$81</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$83</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2351,26 +2375,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -2388,26 +2412,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>419</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>421</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2425,50 +2449,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>428</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>430</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>432</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>434</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>436</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>438</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -2486,34 +2510,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>441</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>443</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>445</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>447</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -2531,66 +2555,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>453</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>456</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>457</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2608,66 +2632,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>456</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>457</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2685,26 +2709,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -2722,10 +2746,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>477</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -2743,26 +2767,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>469</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -2780,18 +2804,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -2801,7 +2825,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3229,6 +3253,14 @@
       </c>
       <c r="B53" t="s" s="0">
         <v>109</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3246,10 +3278,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>382</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3267,50 +3299,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3328,18 +3360,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -3363,30 +3395,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>516</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -3396,7 +3428,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3404,138 +3436,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3553,12 +3593,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3568,7 +3608,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3576,250 +3616,258 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>210</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3829,7 +3877,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3837,650 +3885,666 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>70</v>
+        <v>342</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>339</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>179</v>
+        <v>349</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>180</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>345</v>
+        <v>185</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>346</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="0">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="0">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="0">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="0">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>370</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4498,42 +4562,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>374</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>378</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>382</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -4551,26 +4615,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -4588,50 +4652,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>389</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>391</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>397</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7">
@@ -4639,39 +4703,39 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>399</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>401</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>403</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>405</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>